<commit_message>
add row count and wp-config path
</commit_message>
<xml_diff>
--- a/tests/example-data.xlsx
+++ b/tests/example-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">STOCK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh-10202</t>
   </si>
   <si>
     <t xml:space="preserve">hh-10203</t>
@@ -52,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,7 +134,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -159,8 +157,8 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
+      <c r="B2" s="0" t="n">
+        <v>123</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>9</v>
@@ -171,7 +169,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>5</v>
@@ -182,7 +180,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>4</v>

</xml_diff>